<commit_message>
Revised units for phenol measurements based on reviewer comments
</commit_message>
<xml_diff>
--- a/Phenols/Phenols_graphing_manuscript_25Jan2024.xlsx
+++ b/Phenols/Phenols_graphing_manuscript_25Jan2024.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Academics\UC Davis\School Work\Linquist Lab\Data\R stats\Phenols and 15N\Phenols and 15 Analysis\Phenols\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zhang\Documents\GitHub\15N-and-Phenols-California\Phenols\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -32,12 +32,6 @@
     <t>Field</t>
   </si>
   <si>
-    <t xml:space="preserve">Phenols_level </t>
-  </si>
-  <si>
-    <t>SD</t>
-  </si>
-  <si>
     <t>CR</t>
   </si>
   <si>
@@ -66,6 +60,12 @@
   </si>
   <si>
     <t>Total_phenols</t>
+  </si>
+  <si>
+    <t>Phenols_level_mg_100gOC</t>
+  </si>
+  <si>
+    <t>Phenols_level</t>
   </si>
 </sst>
 </file>
@@ -386,15 +386,15 @@
   <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:E5"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19.140625" customWidth="1"/>
     <col min="3" max="3" width="7.28515625" customWidth="1"/>
-    <col min="4" max="4" width="13.28515625" customWidth="1"/>
-    <col min="5" max="5" width="12" customWidth="1"/>
+    <col min="4" max="4" width="25.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -405,353 +405,353 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" t="s">
         <v>12</v>
       </c>
-      <c r="D1" t="s">
-        <v>2</v>
-      </c>
       <c r="E1" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D2">
         <v>2.2948726847059699</v>
       </c>
       <c r="E2">
-        <v>0.63546961956843695</v>
+        <v>22.948726847059699</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B3" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D3">
         <v>1.9808000467831299</v>
       </c>
       <c r="E3">
-        <v>0.331179499549557</v>
+        <v>19.808000467831299</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B4" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D4">
         <v>1.76065228307114</v>
       </c>
       <c r="E4">
-        <v>0.497623757103894</v>
+        <v>17.606522830711398</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B5" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C5" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D5">
         <v>1.71550511564126</v>
       </c>
       <c r="E5">
-        <v>0.27541929158024903</v>
+        <v>17.1550511564126</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C6" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D6">
         <v>0.21367145420956199</v>
       </c>
       <c r="E6">
-        <v>4.7215912606038302E-2</v>
+        <v>2.13671454209562</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B7" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C7" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D7">
         <v>0.19416448955771101</v>
       </c>
       <c r="E7">
-        <v>3.4632355969068197E-2</v>
+        <v>1.9416448955771102</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B8" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C8" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D8">
         <v>0.18091980014092501</v>
       </c>
       <c r="E8">
-        <v>3.0276815893950201E-2</v>
+        <v>1.8091980014092501</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B9" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C9" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D9">
         <v>0.18883501102146</v>
       </c>
       <c r="E9">
-        <v>2.8464491716621701E-2</v>
+        <v>1.8883501102146001</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B10" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C10" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D10">
         <v>0.58301485634059902</v>
       </c>
       <c r="E10">
-        <v>0.15355670640847699</v>
+        <v>5.8301485634059897</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B11" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C11" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D11">
         <v>0.52765749033582199</v>
       </c>
       <c r="E11">
-        <v>8.9053436277494902E-2</v>
+        <v>5.2765749033582203</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B12" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C12" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D12">
         <v>0.46754972211832602</v>
       </c>
       <c r="E12">
-        <v>0.103878311755587</v>
+        <v>4.6754972211832602</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B13" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C13" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D13">
         <v>0.45834231970392098</v>
       </c>
       <c r="E13">
-        <v>7.4104102608339495E-2</v>
+        <v>4.5834231970392096</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B14" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C14" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D14">
         <v>0.66527396095432101</v>
       </c>
       <c r="E14">
-        <v>0.21838959471935199</v>
+        <v>6.6527396095432101</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B15" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C15" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D15">
         <v>0.58983455243933403</v>
       </c>
       <c r="E15">
-        <v>0.1212403326499</v>
+        <v>5.8983455243933403</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B16" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C16" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D16">
         <v>0.443445151466206</v>
       </c>
       <c r="E16">
-        <v>0.178695743178587</v>
+        <v>4.4344515146620598</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B17" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C17" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D17">
         <v>0.45864148297888302</v>
       </c>
       <c r="E17">
-        <v>0.101879751903403</v>
+        <v>4.5864148297888301</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B18" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C18" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D18">
         <v>0.83291241320148302</v>
       </c>
       <c r="E18">
-        <v>0.24919326104509801</v>
+        <v>8.3291241320148295</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B19" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C19" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D19">
         <v>0.66914351445026399</v>
       </c>
       <c r="E19">
-        <v>9.4854325366602807E-2</v>
+        <v>6.6914351445026394</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B20" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C20" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D20">
         <v>0.66873760934568605</v>
       </c>
       <c r="E20">
-        <v>0.19773852541398401</v>
+        <v>6.6873760934568605</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B21" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C21" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D21">
         <v>0.60968630193699402</v>
       </c>
       <c r="E21">
-        <v>8.9553053527045207E-2</v>
+        <v>6.0968630193699402</v>
       </c>
     </row>
   </sheetData>

</xml_diff>